<commit_message>
new data all duration correlation
</commit_message>
<xml_diff>
--- a/analysis/Summary_Correlations_ConfidenceDifficulty.xlsx
+++ b/analysis/Summary_Correlations_ConfidenceDifficulty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\ML_FaultUnderstanding\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD369C8D-826C-4735-9E73-9A72ED345F0F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FCC197-BCDE-46D1-BA01-3822F91D6E08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13688" windowHeight="4125" activeTab="1" xr2:uid="{3128E891-BECF-4CD7-AE49-319856F740F9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
   <si>
     <t>Professional_Developer</t>
   </si>
@@ -182,6 +182,51 @@
   </si>
   <si>
     <t>p_value: 0.8897930793996093</t>
+  </si>
+  <si>
+    <t>tau: -0.015357223829808038</t>
+  </si>
+  <si>
+    <t>p_value: 0.51891578581743</t>
+  </si>
+  <si>
+    <t>tau: -0.08108201983813217</t>
+  </si>
+  <si>
+    <t>p_value: 0.006762392696709901</t>
+  </si>
+  <si>
+    <t>tau: -0.06409990571883933</t>
+  </si>
+  <si>
+    <t>p_value: 0.15097395421998444</t>
+  </si>
+  <si>
+    <t>tau: -0.09175684097495686</t>
+  </si>
+  <si>
+    <t>p_value: 0.004074214866992513</t>
+  </si>
+  <si>
+    <t>tau: -0.1608537129395914</t>
+  </si>
+  <si>
+    <t>p_value: 0.002441969762034799</t>
+  </si>
+  <si>
+    <t>Non-Significant</t>
+  </si>
+  <si>
+    <t>Weak</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Does not make much difference between all and 1st answer</t>
   </si>
 </sst>
 </file>
@@ -197,12 +242,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -217,8 +292,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,16 +613,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1777DC79-3A70-4171-8F0F-8D9DEEB61836}">
-  <dimension ref="B1:F16"/>
+  <dimension ref="B1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="37.59765625" customWidth="1"/>
-    <col min="3" max="3" width="16.73046875" customWidth="1"/>
+    <col min="3" max="3" width="53.73046875" customWidth="1"/>
     <col min="4" max="4" width="20.73046875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -564,78 +644,133 @@
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
       <c r="C2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
       <c r="C5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C7" t="s">
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
       <c r="C8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
       <c r="C11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C13" t="s">
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
       <c r="C14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C15" t="s">
+      <c r="B15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C16" t="s">
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B19" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -645,17 +780,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A093FFD-DBA1-489D-995C-8DA09363CB39}">
-  <dimension ref="B1:F16"/>
+  <dimension ref="B1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="37.59765625" customWidth="1"/>
-    <col min="3" max="3" width="16.73046875" customWidth="1"/>
-    <col min="4" max="4" width="20.73046875" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.45">
@@ -684,10 +819,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -708,10 +843,10 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -732,10 +867,10 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -756,10 +891,10 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -780,10 +915,10 @@
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -793,6 +928,24 @@
       </c>
       <c r="C16" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>